<commit_message>
json / embeddings / faiss
</commit_message>
<xml_diff>
--- a/data/1038-0610-0614-day.xlsx
+++ b/data/1038-0610-0614-day.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/SustainableSystems/HP_Sustainable_Systems/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFDC3FE7-5BFC-489E-81C9-7033F5E4714C}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC811311-1B1D-4F9A-A37C-F862DE06DFD3}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS-Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
   <si>
     <t>Customer: 1038</t>
   </si>
@@ -409,6 +409,33 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>1.9439301919782395</t>
+  </si>
+  <si>
+    <t>0.8459818930682723</t>
+  </si>
+  <si>
+    <t>9.847564453651831</t>
+  </si>
+  <si>
+    <t>0.8333726182515161</t>
+  </si>
+  <si>
+    <t>2.1842720007002048</t>
+  </si>
+  <si>
+    <t>0.6661471775760394</t>
+  </si>
+  <si>
+    <t>0.8480908716672524</t>
+  </si>
+  <si>
+    <t>3.1831074415286715</t>
+  </si>
+  <si>
+    <t>carbon emissions</t>
   </si>
 </sst>
 </file>
@@ -773,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -865,6 +892,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,6 +908,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1181,14 +1213,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection sqref="A1:BN16"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
@@ -1216,7 +1248,7 @@
     <col min="38" max="43" width="12.28515625" style="1" customWidth="1"/>
     <col min="44" max="44" width="7.5703125" style="1" customWidth="1"/>
     <col min="45" max="45" width="4.42578125" style="1" customWidth="1"/>
-    <col min="46" max="46" width="5.7109375" style="1" customWidth="1"/>
+    <col min="46" max="46" width="17.85546875" style="1" customWidth="1"/>
     <col min="47" max="47" width="9" style="1" customWidth="1"/>
     <col min="48" max="48" width="5.85546875" style="1" customWidth="1"/>
     <col min="49" max="49" width="5.7109375" style="1" customWidth="1"/>
@@ -1274,7 +1306,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>6</v>
@@ -1553,7 +1585,9 @@
       <c r="A6" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="43" t="s">
+        <v>100</v>
+      </c>
       <c r="C6" s="18">
         <v>24</v>
       </c>
@@ -1739,7 +1773,9 @@
       <c r="A7" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="43" t="s">
+        <v>101</v>
+      </c>
       <c r="C7" s="20">
         <v>28</v>
       </c>
@@ -1925,7 +1961,9 @@
       <c r="A8" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="43" t="s">
+        <v>102</v>
+      </c>
       <c r="C8" s="18">
         <v>24</v>
       </c>
@@ -2119,7 +2157,9 @@
       <c r="A9" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="43" t="s">
+        <v>103</v>
+      </c>
       <c r="C9" s="20">
         <v>28</v>
       </c>
@@ -2313,7 +2353,9 @@
       <c r="A10" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="43" t="s">
+        <v>104</v>
+      </c>
       <c r="C10" s="18">
         <v>24</v>
       </c>
@@ -2507,7 +2549,9 @@
       <c r="A11" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="43" t="s">
+        <v>105</v>
+      </c>
       <c r="C11" s="20">
         <v>24</v>
       </c>
@@ -2693,7 +2737,9 @@
       <c r="A12" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="43" t="s">
+        <v>106</v>
+      </c>
       <c r="C12" s="18">
         <v>28</v>
       </c>
@@ -2881,7 +2927,9 @@
       <c r="A13" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="43" t="s">
+        <v>107</v>
+      </c>
       <c r="C13" s="20">
         <v>24</v>
       </c>
@@ -3126,7 +3174,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
WORKING RAG SIMPLIFIED DATA CLOSE TO AUTOMATION
</commit_message>
<xml_diff>
--- a/data/1038-0610-0614-day.xlsx
+++ b/data/1038-0610-0614-day.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC811311-1B1D-4F9A-A37C-F862DE06DFD3}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79740D59-39B0-4F0E-8A62-F723F1761D85}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="750" yWindow="2430" windowWidth="20070" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS-Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="100">
   <si>
     <t>Customer: 1038</t>
   </si>
@@ -409,33 +409,6 @@
   </si>
   <si>
     <t>Avg</t>
-  </si>
-  <si>
-    <t>1.9439301919782395</t>
-  </si>
-  <si>
-    <t>0.8459818930682723</t>
-  </si>
-  <si>
-    <t>9.847564453651831</t>
-  </si>
-  <si>
-    <t>0.8333726182515161</t>
-  </si>
-  <si>
-    <t>2.1842720007002048</t>
-  </si>
-  <si>
-    <t>0.6661471775760394</t>
-  </si>
-  <si>
-    <t>0.8480908716672524</t>
-  </si>
-  <si>
-    <t>3.1831074415286715</t>
-  </si>
-  <si>
-    <t>carbon emissions</t>
   </si>
 </sst>
 </file>
@@ -800,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -854,6 +827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -892,7 +866,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1213,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,20 +1246,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1294,99 +1268,99 @@
       </c>
     </row>
     <row r="3" spans="1:66" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="38" t="s">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="26" t="s">
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="30" t="s">
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="22"/>
-      <c r="AO4" s="22"/>
-      <c r="AP4" s="22"/>
-      <c r="AQ4" s="23"/>
-      <c r="AR4" s="28" t="s">
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="23"/>
+      <c r="AN4" s="23"/>
+      <c r="AO4" s="23"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="25"/>
-      <c r="AU4" s="25"/>
-      <c r="AV4" s="25"/>
-      <c r="AW4" s="25"/>
-      <c r="AX4" s="25"/>
-      <c r="AY4" s="29"/>
-      <c r="AZ4" s="24" t="s">
+      <c r="AS4" s="26"/>
+      <c r="AT4" s="26"/>
+      <c r="AU4" s="26"/>
+      <c r="AV4" s="26"/>
+      <c r="AW4" s="26"/>
+      <c r="AX4" s="26"/>
+      <c r="AY4" s="30"/>
+      <c r="AZ4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="BA4" s="25"/>
-      <c r="BB4" s="25"/>
-      <c r="BC4" s="25"/>
-      <c r="BD4" s="25"/>
-      <c r="BE4" s="25"/>
-      <c r="BF4" s="25"/>
-      <c r="BG4" s="25"/>
-      <c r="BH4" s="25"/>
-      <c r="BI4" s="25"/>
-      <c r="BJ4" s="25"/>
-      <c r="BK4" s="25"/>
-      <c r="BL4" s="25"/>
-      <c r="BM4" s="25"/>
-      <c r="BN4" s="25"/>
+      <c r="BA4" s="26"/>
+      <c r="BB4" s="26"/>
+      <c r="BC4" s="26"/>
+      <c r="BD4" s="26"/>
+      <c r="BE4" s="26"/>
+      <c r="BF4" s="26"/>
+      <c r="BG4" s="26"/>
+      <c r="BH4" s="26"/>
+      <c r="BI4" s="26"/>
+      <c r="BJ4" s="26"/>
+      <c r="BK4" s="26"/>
+      <c r="BL4" s="26"/>
+      <c r="BM4" s="26"/>
+      <c r="BN4" s="26"/>
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="32"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
@@ -1585,9 +1559,7 @@
       <c r="A6" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="43" t="s">
-        <v>100</v>
-      </c>
+      <c r="B6" s="21"/>
       <c r="C6" s="18">
         <v>24</v>
       </c>
@@ -1773,9 +1745,7 @@
       <c r="A7" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>101</v>
-      </c>
+      <c r="B7" s="21"/>
       <c r="C7" s="20">
         <v>28</v>
       </c>
@@ -1961,9 +1931,7 @@
       <c r="A8" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="43" t="s">
-        <v>102</v>
-      </c>
+      <c r="B8" s="21"/>
       <c r="C8" s="18">
         <v>24</v>
       </c>
@@ -2157,9 +2125,7 @@
       <c r="A9" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>103</v>
-      </c>
+      <c r="B9" s="21"/>
       <c r="C9" s="20">
         <v>28</v>
       </c>
@@ -2353,9 +2319,7 @@
       <c r="A10" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="43" t="s">
-        <v>104</v>
-      </c>
+      <c r="B10" s="21"/>
       <c r="C10" s="18">
         <v>24</v>
       </c>
@@ -2549,9 +2513,7 @@
       <c r="A11" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>105</v>
-      </c>
+      <c r="B11" s="21"/>
       <c r="C11" s="20">
         <v>24</v>
       </c>
@@ -2737,9 +2699,7 @@
       <c r="A12" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="43" t="s">
-        <v>106</v>
-      </c>
+      <c r="B12" s="21"/>
       <c r="C12" s="18">
         <v>28</v>
       </c>
@@ -2927,9 +2887,7 @@
       <c r="A13" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="43" t="s">
-        <v>107</v>
-      </c>
+      <c r="B13" s="21"/>
       <c r="C13" s="20">
         <v>24</v>
       </c>
@@ -3215,20 +3173,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3237,57 +3195,57 @@
       </c>
     </row>
     <row r="3" spans="1:66" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="38" t="s">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="26" t="s">
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="27"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="28"/>
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -3644,20 +3602,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3666,12 +3624,12 @@
       </c>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3736,26 +3694,26 @@
       <c r="BN3" s="1"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="41" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="42" t="s">
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="14" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
got time window in
</commit_message>
<xml_diff>
--- a/data/1038-0610-0614-day.xlsx
+++ b/data/1038-0610-0614-day.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucabmr3_ucl_ac_uk/Documents/UCL_comp_sci/Sustainable_Systems_3/HP_Sus_Sys_3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79740D59-39B0-4F0E-8A62-F723F1761D85}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_79DA2B6B5C3787F24A9A54D881E28314B5F12F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E69C97D-66A1-4395-86F7-B7D7128EAF13}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="750" yWindow="2430" windowWidth="20070" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="11970" windowHeight="8370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS-Data" sheetId="1" r:id="rId1"/>
@@ -846,8 +846,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,6 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -866,7 +867,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,7 +1188,7 @@
   <dimension ref="A1:BN16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1279,7 @@
       <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="32" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="34" t="s">
@@ -1361,7 +1361,7 @@
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="38"/>
-      <c r="B5" s="32"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -3206,7 +3206,7 @@
       <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="34" t="s">
@@ -3245,7 +3245,7 @@
     </row>
     <row r="5" spans="1:66" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="38"/>
-      <c r="B5" s="33"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
@@ -3694,26 +3694,26 @@
       <c r="BN3" s="1"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>91</v>
       </c>
       <c r="C4" s="36"/>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="43" t="s">
         <v>92</v>
       </c>
       <c r="E4" s="35"/>
       <c r="F4" s="36"/>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="44" t="s">
         <v>93</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="14" t="s">
         <v>94</v>
       </c>

</xml_diff>